<commit_message>
A first version of the major revised paper for JSTSP
</commit_message>
<xml_diff>
--- a/paper_writing/JSTSP/revision/new_charts.xlsx
+++ b/paper_writing/JSTSP/revision/new_charts.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961B4F17-B8AF-4FCC-A8FA-8AC968229EE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D998405B-2ADF-437D-8EDA-88553D9968E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perception_v0_v1" sheetId="1" r:id="rId1"/>
@@ -298,9 +298,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -313,6 +310,9 @@
     </xf>
     <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3725,6 +3725,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -7588,18 +7619,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -7877,18 +7908,18 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -8574,7 +8605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41931C90-4707-4D32-9771-4E5DE4848207}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8656,8 +8689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF8ABB1-1175-4983-BF00-9A9881D7B9B1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N58" sqref="N58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8671,7 +8704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA922B0E-6C1D-47B5-92AE-0D65695F4E55}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -8690,7 +8723,7 @@
     </row>
     <row r="2" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
-      <c r="B2" s="28"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="33" t="s">
         <v>18</v>
       </c>
@@ -8700,105 +8733,105 @@
     </row>
     <row r="3" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="28">
         <v>1</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>2</v>
       </c>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <v>3</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
-      <c r="B4" s="29">
+      <c r="B4" s="28">
         <v>500</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>0.947075</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>0.72155000000000002</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>0.13694300000000001</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="29">
         <v>2.1661E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
-      <c r="B5" s="29">
+      <c r="B5" s="28">
         <v>1000</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>0.93674000000000002</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>0.83736299999999997</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>0.30555599999999999</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="29">
         <v>6.2801999999999997E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>2000</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>0.95852499999999996</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>0.86714999999999998</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="29">
         <v>0.382716</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="29">
         <v>0.13573399999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
-      <c r="B7" s="29">
+      <c r="B7" s="28">
         <v>5000</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>0.96474400000000005</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>0.83423899999999995</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>0.52390400000000004</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <v>0.28821000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
-      <c r="B9" s="29"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="33" t="s">
         <v>19</v>
       </c>
@@ -8808,89 +8841,89 @@
     </row>
     <row r="10" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>1</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>2</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>3</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
-      <c r="B11" s="29">
+      <c r="B11" s="28">
         <v>500</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="29">
         <v>0.95584400000000003</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="29">
         <v>0.83564799999999995</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="29">
         <v>5.3254000000000003E-2</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="29">
         <v>1.2987E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="29">
+      <c r="B12" s="28">
         <v>1000</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <v>0.95324699999999996</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <v>0.90129899999999996</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>0.201183</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="29">
         <v>3.9351999999999998E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="29">
+      <c r="B13" s="28">
         <v>2000</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="29">
         <v>0.962422</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="29">
         <v>0.90909099999999998</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="29">
         <v>0.45704499999999998</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <v>0.14026</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="29">
+      <c r="B14" s="28">
         <v>5000</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="29">
         <v>0.98224900000000004</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="29">
         <v>0.91752599999999995</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="29">
         <v>0.64155799999999996</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="29">
         <v>0.24904899999999999</v>
       </c>
     </row>

</xml_diff>